<commit_message>
Added 3D models, updated U11 (AD5254), fixed footprints, updated libraries, schematics and project files.
</commit_message>
<xml_diff>
--- a/Project Outputs for fader2_pcb/BOM/Bill of Materials-fader2_pcb.xlsx
+++ b/Project Outputs for fader2_pcb/BOM/Bill of Materials-fader2_pcb.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caolen\Nokia\Fader2.5\fader25_pcb\Project Outputs for fader2_pcb\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF74B5CD-58C1-411F-9A49-D9AEF91E7D1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4628" windowHeight="10628"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="2175" windowWidth="25815" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-fader2_pcb" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -756,7 +768,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1099,17 +1111,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="6.796875" customWidth="1"/>
+    <col min="1" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="10" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1173,7 +1189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1205,7 +1221,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1237,7 +1253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1269,7 +1285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1301,7 +1317,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -1333,7 +1349,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -1365,7 +1381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1397,7 +1413,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>62</v>
       </c>
@@ -1429,7 +1445,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>67</v>
       </c>
@@ -1461,7 +1477,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>72</v>
       </c>
@@ -1493,7 +1509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>78</v>
       </c>
@@ -1525,7 +1541,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>84</v>
       </c>
@@ -1557,7 +1573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>91</v>
       </c>
@@ -1589,7 +1605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>96</v>
       </c>
@@ -1621,7 +1637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>102</v>
       </c>
@@ -1653,7 +1669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>108</v>
       </c>
@@ -1685,7 +1701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -1717,7 +1733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>119</v>
       </c>
@@ -1749,7 +1765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>126</v>
       </c>
@@ -1781,7 +1797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>131</v>
       </c>
@@ -1813,7 +1829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>136</v>
       </c>
@@ -1845,7 +1861,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>141</v>
       </c>
@@ -1877,7 +1893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>146</v>
       </c>
@@ -1909,7 +1925,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>151</v>
       </c>
@@ -1941,7 +1957,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>156</v>
       </c>
@@ -1973,7 +1989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>161</v>
       </c>
@@ -2005,7 +2021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>166</v>
       </c>
@@ -2037,7 +2053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>171</v>
       </c>
@@ -2069,7 +2085,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>176</v>
       </c>
@@ -2101,7 +2117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>184</v>
       </c>
@@ -2133,7 +2149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>191</v>
       </c>
@@ -2165,7 +2181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>13</v>
       </c>
@@ -2197,7 +2213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>198</v>
       </c>
@@ -2229,7 +2245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>13</v>
       </c>
@@ -2261,7 +2277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>206</v>
       </c>
@@ -2293,7 +2309,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>212</v>
       </c>
@@ -2325,7 +2341,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>219</v>
       </c>
@@ -2357,7 +2373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>224</v>
       </c>
@@ -2389,7 +2405,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>230</v>
       </c>
@@ -2421,7 +2437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>237</v>
       </c>

</xml_diff>